<commit_message>
Implement income parsing for a new report type
</commit_message>
<xml_diff>
--- a/InvestmentReporting.UnitTests/Samples/Tinkoff_BrokerMoneyMove_IncomeSample.xlsx
+++ b/InvestmentReporting.UnitTests/Samples/Tinkoff_BrokerMoneyMove_IncomeSample.xlsx
@@ -11,27 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
-  <si>
-    <t xml:space="preserve">
-Брокер: АО «Тинькофф Банк», ИНН/КПП 7710140679/773401001
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Дата расчета: 01.03.2000
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Инвестор: ИВАНОВ ИВАН ИВАНОВИЧ / 0000000000 от 01.01.2000
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Отчет о сделках и операциях за период 01.01.2000 - 02.01.2000
-</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
   <si>
     <t xml:space="preserve">
 1.1 Информация о совершенных и исполненных сделках на конец отчетного периода
@@ -712,16 +692,8 @@
   </si>
   <si>
     <t xml:space="preserve">
-Руководитель отдела брокерских услуг:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
 Подпись:
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Сотрудник банка, ответственный за ведение внутреннего учета (ФИО):</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -738,7 +710,7 @@
     <numFmt numFmtId="59" formatCode="dd.mm.yyyy"/>
     <numFmt numFmtId="60" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -783,11 +755,6 @@
       <sz val="4"/>
       <color indexed="8"/>
       <name val="Neue_Haas"/>
-    </font>
-    <font>
-      <sz val="5"/>
-      <color indexed="8"/>
-      <name val="DejaVu Sans"/>
     </font>
     <font>
       <sz val="6"/>
@@ -1417,31 +1384,31 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1465,34 +1432,34 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="9" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="7" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="9" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="7" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="9" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="7" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="9" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="7" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1522,16 +1489,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1546,28 +1513,28 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1588,25 +1555,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="38" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1837,13 +1804,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -1942,10 +1903,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2200,13 +2161,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -2519,10 +2474,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3004,9 +2959,7 @@
       <c r="EW1" s="2"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>0</v>
-      </c>
+      <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3161,9 +3114,7 @@
       <c r="EW2" s="4"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="3">
-        <v>1</v>
-      </c>
+      <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -3473,9 +3424,7 @@
       <c r="EW4" s="6"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="7">
-        <v>2</v>
-      </c>
+      <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -3630,9 +3579,7 @@
       <c r="EW5" s="9"/>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="10">
-        <v>3</v>
-      </c>
+      <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -3788,7 +3735,7 @@
     </row>
     <row r="7" ht="25" customHeight="1">
       <c r="A7" t="s" s="13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -3945,24 +3892,24 @@
     </row>
     <row r="8" ht="40" customHeight="1">
       <c r="A8" t="s" s="16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" t="s" s="18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
       <c r="H8" t="s" s="18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
       <c r="L8" t="s" s="18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
@@ -3970,7 +3917,7 @@
       <c r="P8" s="19"/>
       <c r="Q8" s="19"/>
       <c r="R8" t="s" s="18">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="S8" s="19"/>
       <c r="T8" s="19"/>
@@ -3978,19 +3925,19 @@
       <c r="V8" s="19"/>
       <c r="W8" s="19"/>
       <c r="X8" t="s" s="18">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Y8" s="19"/>
       <c r="Z8" s="19"/>
       <c r="AA8" s="19"/>
       <c r="AB8" t="s" s="18">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AC8" s="19"/>
       <c r="AD8" s="19"/>
       <c r="AE8" s="19"/>
       <c r="AF8" t="s" s="18">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AG8" s="19"/>
       <c r="AH8" s="19"/>
@@ -4000,39 +3947,39 @@
       <c r="AL8" s="19"/>
       <c r="AM8" s="19"/>
       <c r="AN8" t="s" s="18">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
       <c r="AQ8" s="19"/>
       <c r="AR8" s="19"/>
       <c r="AS8" t="s" s="18">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AT8" s="19"/>
       <c r="AU8" s="19"/>
       <c r="AV8" s="19"/>
       <c r="AW8" t="s" s="18">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AX8" s="19"/>
       <c r="AY8" s="19"/>
       <c r="AZ8" s="19"/>
       <c r="BA8" s="19"/>
       <c r="BB8" t="s" s="18">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="BC8" s="19"/>
       <c r="BD8" s="19"/>
       <c r="BE8" t="s" s="18">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="BF8" s="19"/>
       <c r="BG8" s="19"/>
       <c r="BH8" s="19"/>
       <c r="BI8" s="19"/>
       <c r="BJ8" t="s" s="18">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="BK8" s="19"/>
       <c r="BL8" s="19"/>
@@ -4041,7 +3988,7 @@
       <c r="BO8" s="19"/>
       <c r="BP8" s="19"/>
       <c r="BQ8" t="s" s="18">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="BR8" s="19"/>
       <c r="BS8" s="19"/>
@@ -4049,7 +3996,7 @@
       <c r="BU8" s="19"/>
       <c r="BV8" s="19"/>
       <c r="BW8" t="s" s="18">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="BX8" s="19"/>
       <c r="BY8" s="19"/>
@@ -4057,27 +4004,27 @@
       <c r="CA8" s="19"/>
       <c r="CB8" s="19"/>
       <c r="CC8" t="s" s="18">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="CD8" s="19"/>
       <c r="CE8" s="19"/>
       <c r="CF8" s="19"/>
       <c r="CG8" t="s" s="18">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="CH8" s="19"/>
       <c r="CI8" s="19"/>
       <c r="CJ8" s="19"/>
       <c r="CK8" s="19"/>
       <c r="CL8" t="s" s="18">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="CM8" s="19"/>
       <c r="CN8" s="19"/>
       <c r="CO8" s="19"/>
       <c r="CP8" s="19"/>
       <c r="CQ8" t="s" s="18">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="CR8" s="19"/>
       <c r="CS8" s="19"/>
@@ -4085,32 +4032,32 @@
       <c r="CU8" s="19"/>
       <c r="CV8" s="19"/>
       <c r="CW8" t="s" s="18">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="CX8" s="19"/>
       <c r="CY8" s="19"/>
       <c r="CZ8" s="19"/>
       <c r="DA8" t="s" s="18">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="DB8" s="19"/>
       <c r="DC8" s="19"/>
       <c r="DD8" s="19"/>
       <c r="DE8" t="s" s="18">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="DF8" s="19"/>
       <c r="DG8" s="19"/>
       <c r="DH8" s="19"/>
       <c r="DI8" s="19"/>
       <c r="DJ8" t="s" s="18">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="DK8" s="19"/>
       <c r="DL8" s="19"/>
       <c r="DM8" s="19"/>
       <c r="DN8" t="s" s="18">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="DO8" s="19"/>
       <c r="DP8" s="19"/>
@@ -4118,7 +4065,7 @@
       <c r="DR8" s="19"/>
       <c r="DS8" s="19"/>
       <c r="DT8" t="s" s="18">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="DU8" s="19"/>
       <c r="DV8" s="19"/>
@@ -4126,7 +4073,7 @@
       <c r="DX8" s="19"/>
       <c r="DY8" s="19"/>
       <c r="DZ8" t="s" s="18">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="EA8" s="19"/>
       <c r="EB8" s="19"/>
@@ -4134,27 +4081,27 @@
       <c r="ED8" s="19"/>
       <c r="EE8" s="19"/>
       <c r="EF8" t="s" s="18">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="EG8" s="19"/>
       <c r="EH8" s="19"/>
       <c r="EI8" s="19"/>
       <c r="EJ8" s="19"/>
       <c r="EK8" t="s" s="18">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="EL8" s="19"/>
       <c r="EM8" s="19"/>
       <c r="EN8" s="19"/>
       <c r="EO8" s="19"/>
       <c r="EP8" t="s" s="18">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="EQ8" s="19"/>
       <c r="ER8" s="19"/>
       <c r="ES8" s="19"/>
       <c r="ET8" t="s" s="18">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="EU8" s="19"/>
       <c r="EV8" s="19"/>
@@ -4162,7 +4109,7 @@
     </row>
     <row r="9" ht="25" customHeight="1">
       <c r="A9" t="s" s="21">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
@@ -4319,25 +4266,25 @@
     </row>
     <row r="10" ht="40" customHeight="1">
       <c r="A10" t="s" s="25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" t="s" s="18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" t="s" s="18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" t="s" s="18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
@@ -4346,7 +4293,7 @@
       <c r="R10" s="19"/>
       <c r="S10" s="19"/>
       <c r="T10" t="s" s="18">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="U10" s="19"/>
       <c r="V10" s="19"/>
@@ -4354,19 +4301,19 @@
       <c r="X10" s="19"/>
       <c r="Y10" s="19"/>
       <c r="Z10" t="s" s="18">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AA10" s="19"/>
       <c r="AB10" s="19"/>
       <c r="AC10" s="19"/>
       <c r="AD10" t="s" s="18">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AE10" s="19"/>
       <c r="AF10" s="19"/>
       <c r="AG10" s="19"/>
       <c r="AH10" t="s" s="18">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AI10" s="19"/>
       <c r="AJ10" s="19"/>
@@ -4376,39 +4323,39 @@
       <c r="AN10" s="19"/>
       <c r="AO10" s="19"/>
       <c r="AP10" t="s" s="18">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AQ10" s="19"/>
       <c r="AR10" s="19"/>
       <c r="AS10" s="19"/>
       <c r="AT10" s="19"/>
       <c r="AU10" t="s" s="18">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AV10" s="19"/>
       <c r="AW10" s="19"/>
       <c r="AX10" s="19"/>
       <c r="AY10" t="s" s="18">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AZ10" s="19"/>
       <c r="BA10" s="19"/>
       <c r="BB10" s="19"/>
       <c r="BC10" s="19"/>
       <c r="BD10" t="s" s="18">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="BE10" s="19"/>
       <c r="BF10" s="19"/>
       <c r="BG10" t="s" s="18">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="BH10" s="19"/>
       <c r="BI10" s="19"/>
       <c r="BJ10" s="19"/>
       <c r="BK10" s="19"/>
       <c r="BL10" t="s" s="18">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="BM10" s="19"/>
       <c r="BN10" s="19"/>
@@ -4417,7 +4364,7 @@
       <c r="BQ10" s="19"/>
       <c r="BR10" s="19"/>
       <c r="BS10" t="s" s="18">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="BT10" s="19"/>
       <c r="BU10" s="19"/>
@@ -4425,7 +4372,7 @@
       <c r="BW10" s="19"/>
       <c r="BX10" s="19"/>
       <c r="BY10" t="s" s="18">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="BZ10" s="19"/>
       <c r="CA10" s="19"/>
@@ -4433,27 +4380,27 @@
       <c r="CC10" s="19"/>
       <c r="CD10" s="19"/>
       <c r="CE10" t="s" s="18">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="CF10" s="19"/>
       <c r="CG10" s="19"/>
       <c r="CH10" s="19"/>
       <c r="CI10" t="s" s="18">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="CJ10" s="19"/>
       <c r="CK10" s="19"/>
       <c r="CL10" s="19"/>
       <c r="CM10" s="19"/>
       <c r="CN10" t="s" s="18">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="CO10" s="19"/>
       <c r="CP10" s="19"/>
       <c r="CQ10" s="19"/>
       <c r="CR10" s="19"/>
       <c r="CS10" t="s" s="18">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="CT10" s="19"/>
       <c r="CU10" s="19"/>
@@ -4461,32 +4408,32 @@
       <c r="CW10" s="19"/>
       <c r="CX10" s="19"/>
       <c r="CY10" t="s" s="18">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="CZ10" s="19"/>
       <c r="DA10" s="19"/>
       <c r="DB10" s="19"/>
       <c r="DC10" t="s" s="18">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="DD10" s="19"/>
       <c r="DE10" s="19"/>
       <c r="DF10" s="19"/>
       <c r="DG10" t="s" s="18">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="DH10" s="19"/>
       <c r="DI10" s="19"/>
       <c r="DJ10" s="19"/>
       <c r="DK10" s="19"/>
       <c r="DL10" t="s" s="18">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="DM10" s="19"/>
       <c r="DN10" s="19"/>
       <c r="DO10" s="19"/>
       <c r="DP10" t="s" s="18">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="DQ10" s="19"/>
       <c r="DR10" s="19"/>
@@ -4494,7 +4441,7 @@
       <c r="DT10" s="19"/>
       <c r="DU10" s="19"/>
       <c r="DV10" t="s" s="18">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="DW10" s="19"/>
       <c r="DX10" s="19"/>
@@ -4502,7 +4449,7 @@
       <c r="DZ10" s="19"/>
       <c r="EA10" s="19"/>
       <c r="EB10" t="s" s="18">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="EC10" s="19"/>
       <c r="ED10" s="19"/>
@@ -4511,32 +4458,32 @@
       <c r="EG10" s="19"/>
       <c r="EH10" s="19"/>
       <c r="EI10" t="s" s="18">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="EJ10" s="19"/>
       <c r="EK10" s="19"/>
       <c r="EL10" s="19"/>
       <c r="EM10" s="19"/>
       <c r="EN10" t="s" s="18">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="EO10" s="19"/>
       <c r="EP10" s="19"/>
       <c r="EQ10" s="19"/>
       <c r="ER10" t="s" s="18">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="ES10" s="19"/>
       <c r="ET10" s="19"/>
       <c r="EU10" s="19"/>
       <c r="EV10" s="19"/>
       <c r="EW10" t="s" s="26">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" ht="25" customHeight="1">
       <c r="A11" t="s" s="27">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -4693,24 +4640,24 @@
     </row>
     <row r="12" ht="40" customHeight="1">
       <c r="A12" t="s" s="25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" t="s" s="18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" t="s" s="18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="L12" t="s" s="18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
@@ -4719,7 +4666,7 @@
       <c r="Q12" s="19"/>
       <c r="R12" s="19"/>
       <c r="S12" t="s" s="18">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="T12" s="19"/>
       <c r="U12" s="19"/>
@@ -4727,19 +4674,19 @@
       <c r="W12" s="19"/>
       <c r="X12" s="19"/>
       <c r="Y12" t="s" s="18">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Z12" s="19"/>
       <c r="AA12" s="19"/>
       <c r="AB12" s="19"/>
       <c r="AC12" t="s" s="18">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AD12" s="19"/>
       <c r="AE12" s="19"/>
       <c r="AF12" s="19"/>
       <c r="AG12" t="s" s="18">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AH12" s="19"/>
       <c r="AI12" s="19"/>
@@ -4749,39 +4696,39 @@
       <c r="AM12" s="19"/>
       <c r="AN12" s="19"/>
       <c r="AO12" t="s" s="18">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AP12" s="19"/>
       <c r="AQ12" s="19"/>
       <c r="AR12" s="19"/>
       <c r="AS12" s="19"/>
       <c r="AT12" t="s" s="18">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AU12" s="19"/>
       <c r="AV12" s="19"/>
       <c r="AW12" s="19"/>
       <c r="AX12" t="s" s="18">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AY12" s="19"/>
       <c r="AZ12" s="19"/>
       <c r="BA12" s="19"/>
       <c r="BB12" s="19"/>
       <c r="BC12" t="s" s="18">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="BD12" s="19"/>
       <c r="BE12" s="19"/>
       <c r="BF12" t="s" s="18">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="BG12" s="19"/>
       <c r="BH12" s="19"/>
       <c r="BI12" s="19"/>
       <c r="BJ12" s="19"/>
       <c r="BK12" t="s" s="18">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="BL12" s="19"/>
       <c r="BM12" s="19"/>
@@ -4790,7 +4737,7 @@
       <c r="BP12" s="19"/>
       <c r="BQ12" s="19"/>
       <c r="BR12" t="s" s="18">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="BS12" s="19"/>
       <c r="BT12" s="19"/>
@@ -4798,7 +4745,7 @@
       <c r="BV12" s="19"/>
       <c r="BW12" s="19"/>
       <c r="BX12" t="s" s="18">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="BY12" s="19"/>
       <c r="BZ12" s="19"/>
@@ -4806,27 +4753,27 @@
       <c r="CB12" s="19"/>
       <c r="CC12" s="19"/>
       <c r="CD12" t="s" s="18">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="CE12" s="19"/>
       <c r="CF12" s="19"/>
       <c r="CG12" s="19"/>
       <c r="CH12" t="s" s="18">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="CI12" s="19"/>
       <c r="CJ12" s="19"/>
       <c r="CK12" s="19"/>
       <c r="CL12" s="19"/>
       <c r="CM12" t="s" s="18">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="CN12" s="19"/>
       <c r="CO12" s="19"/>
       <c r="CP12" s="19"/>
       <c r="CQ12" s="19"/>
       <c r="CR12" t="s" s="18">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="CS12" s="19"/>
       <c r="CT12" s="19"/>
@@ -4834,32 +4781,32 @@
       <c r="CV12" s="19"/>
       <c r="CW12" s="19"/>
       <c r="CX12" t="s" s="18">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="CY12" s="19"/>
       <c r="CZ12" s="19"/>
       <c r="DA12" s="19"/>
       <c r="DB12" t="s" s="18">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="DC12" s="19"/>
       <c r="DD12" s="19"/>
       <c r="DE12" s="19"/>
       <c r="DF12" t="s" s="18">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="DG12" s="19"/>
       <c r="DH12" s="19"/>
       <c r="DI12" s="19"/>
       <c r="DJ12" s="19"/>
       <c r="DK12" t="s" s="18">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="DL12" s="19"/>
       <c r="DM12" s="19"/>
       <c r="DN12" s="19"/>
       <c r="DO12" t="s" s="18">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="DP12" s="19"/>
       <c r="DQ12" s="19"/>
@@ -4867,7 +4814,7 @@
       <c r="DS12" s="19"/>
       <c r="DT12" s="19"/>
       <c r="DU12" t="s" s="18">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="DV12" s="19"/>
       <c r="DW12" s="19"/>
@@ -4875,7 +4822,7 @@
       <c r="DY12" s="19"/>
       <c r="DZ12" s="19"/>
       <c r="EA12" t="s" s="18">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="EB12" s="19"/>
       <c r="EC12" s="19"/>
@@ -4884,27 +4831,27 @@
       <c r="EF12" s="19"/>
       <c r="EG12" s="19"/>
       <c r="EH12" t="s" s="18">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="EI12" s="19"/>
       <c r="EJ12" s="19"/>
       <c r="EK12" s="19"/>
       <c r="EL12" t="s" s="18">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="EM12" s="19"/>
       <c r="EN12" s="19"/>
       <c r="EO12" s="19"/>
       <c r="EP12" s="19"/>
       <c r="EQ12" t="s" s="18">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="ER12" s="19"/>
       <c r="ES12" s="19"/>
       <c r="ET12" s="19"/>
       <c r="EU12" s="19"/>
       <c r="EV12" t="s" s="18">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="EW12" s="20"/>
     </row>
@@ -5054,7 +5001,7 @@
       <c r="EM13" s="28"/>
       <c r="EN13" s="28"/>
       <c r="EO13" t="s" s="29">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="EP13" s="30"/>
       <c r="EQ13" s="30"/>
@@ -5069,7 +5016,7 @@
     </row>
     <row r="14" ht="25" customHeight="1">
       <c r="A14" t="s" s="13">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -5226,25 +5173,25 @@
     </row>
     <row r="15" ht="53" customHeight="1">
       <c r="A15" t="s" s="25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" t="s" s="18">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="F15" t="s" s="18">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" t="s" s="18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J15" s="19"/>
       <c r="K15" t="s" s="18">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
@@ -5256,7 +5203,7 @@
       <c r="S15" s="19"/>
       <c r="T15" s="19"/>
       <c r="U15" t="s" s="18">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="V15" s="19"/>
       <c r="W15" s="19"/>
@@ -5264,13 +5211,13 @@
       <c r="Y15" s="19"/>
       <c r="Z15" s="19"/>
       <c r="AA15" t="s" s="18">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
       <c r="AD15" s="19"/>
       <c r="AE15" t="s" s="18">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AF15" s="19"/>
       <c r="AG15" s="19"/>
@@ -5279,31 +5226,31 @@
       <c r="AJ15" s="19"/>
       <c r="AK15" s="19"/>
       <c r="AL15" t="s" s="18">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AM15" s="19"/>
       <c r="AN15" s="19"/>
       <c r="AO15" s="19"/>
       <c r="AP15" s="19"/>
       <c r="AQ15" t="s" s="18">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AR15" s="19"/>
       <c r="AS15" t="s" s="18">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AT15" s="19"/>
       <c r="AU15" s="19"/>
       <c r="AV15" s="19"/>
       <c r="AW15" t="s" s="18">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AX15" s="19"/>
       <c r="AY15" s="19"/>
       <c r="AZ15" s="19"/>
       <c r="BA15" s="19"/>
       <c r="BB15" t="s" s="18">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="BC15" s="19"/>
       <c r="BD15" s="19"/>
@@ -5311,14 +5258,14 @@
       <c r="BF15" s="19"/>
       <c r="BG15" s="19"/>
       <c r="BH15" t="s" s="18">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="BI15" s="19"/>
       <c r="BJ15" s="19"/>
       <c r="BK15" s="19"/>
       <c r="BL15" s="19"/>
       <c r="BM15" t="s" s="18">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="BN15" s="19"/>
       <c r="BO15" s="19"/>
@@ -5327,7 +5274,7 @@
       <c r="BR15" s="19"/>
       <c r="BS15" s="19"/>
       <c r="BT15" t="s" s="18">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="BU15" s="19"/>
       <c r="BV15" s="19"/>
@@ -5336,21 +5283,21 @@
       <c r="BY15" s="19"/>
       <c r="BZ15" s="19"/>
       <c r="CA15" t="s" s="18">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CB15" s="19"/>
       <c r="CC15" s="19"/>
       <c r="CD15" s="19"/>
       <c r="CE15" s="19"/>
       <c r="CF15" t="s" s="18">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="CG15" s="19"/>
       <c r="CH15" s="19"/>
       <c r="CI15" s="19"/>
       <c r="CJ15" s="19"/>
       <c r="CK15" t="s" s="18">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="CL15" s="19"/>
       <c r="CM15" s="19"/>
@@ -5361,7 +5308,7 @@
       <c r="CR15" s="19"/>
       <c r="CS15" s="19"/>
       <c r="CT15" t="s" s="18">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="CU15" s="19"/>
       <c r="CV15" s="19"/>
@@ -5373,14 +5320,14 @@
       <c r="DB15" s="19"/>
       <c r="DC15" s="19"/>
       <c r="DD15" t="s" s="18">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="DE15" s="19"/>
       <c r="DF15" s="19"/>
       <c r="DG15" s="19"/>
       <c r="DH15" s="19"/>
       <c r="DI15" t="s" s="18">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="DJ15" s="19"/>
       <c r="DK15" s="19"/>
@@ -5391,7 +5338,7 @@
       <c r="DP15" s="19"/>
       <c r="DQ15" s="19"/>
       <c r="DR15" t="s" s="18">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="DS15" s="19"/>
       <c r="DT15" s="19"/>
@@ -5399,14 +5346,14 @@
       <c r="DV15" s="19"/>
       <c r="DW15" s="19"/>
       <c r="DX15" t="s" s="18">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="DY15" s="19"/>
       <c r="DZ15" s="19"/>
       <c r="EA15" s="19"/>
       <c r="EB15" s="19"/>
       <c r="EC15" t="s" s="18">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="ED15" s="19"/>
       <c r="EE15" s="19"/>
@@ -5418,7 +5365,7 @@
       <c r="EK15" s="19"/>
       <c r="EL15" s="19"/>
       <c r="EM15" t="s" s="18">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="EN15" s="19"/>
       <c r="EO15" s="19"/>
@@ -5428,7 +5375,7 @@
       <c r="ES15" s="19"/>
       <c r="ET15" s="19"/>
       <c r="EU15" t="s" s="18">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="EV15" s="19"/>
       <c r="EW15" s="20"/>
@@ -5590,7 +5537,7 @@
     </row>
     <row r="17" ht="25" customHeight="1">
       <c r="A17" t="s" s="27">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -5747,7 +5694,7 @@
     </row>
     <row r="18" ht="40" customHeight="1">
       <c r="A18" t="s" s="36">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -5762,7 +5709,7 @@
       <c r="L18" s="37"/>
       <c r="M18" s="37"/>
       <c r="N18" t="s" s="38">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="O18" s="37"/>
       <c r="P18" s="37"/>
@@ -5783,7 +5730,7 @@
       <c r="AE18" s="37"/>
       <c r="AF18" s="37"/>
       <c r="AG18" t="s" s="38">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="AH18" s="37"/>
       <c r="AI18" s="37"/>
@@ -5804,7 +5751,7 @@
       <c r="AX18" s="37"/>
       <c r="AY18" s="37"/>
       <c r="AZ18" t="s" s="38">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="BA18" s="37"/>
       <c r="BB18" s="37"/>
@@ -5828,7 +5775,7 @@
       <c r="BT18" s="37"/>
       <c r="BU18" s="37"/>
       <c r="BV18" t="s" s="38">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="BW18" s="37"/>
       <c r="BX18" s="37"/>
@@ -5853,7 +5800,7 @@
       <c r="CQ18" s="37"/>
       <c r="CR18" s="37"/>
       <c r="CS18" t="s" s="38">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="CT18" s="37"/>
       <c r="CU18" s="37"/>
@@ -5879,7 +5826,7 @@
       <c r="DO18" s="37"/>
       <c r="DP18" s="37"/>
       <c r="DQ18" t="s" s="38">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="DR18" s="37"/>
       <c r="DS18" s="37"/>
@@ -5916,7 +5863,7 @@
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="40">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
@@ -5931,7 +5878,7 @@
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
       <c r="N19" t="s" s="42">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O19" s="41"/>
       <c r="P19" s="41"/>
@@ -5997,7 +5944,7 @@
       <c r="BT19" s="41"/>
       <c r="BU19" s="41"/>
       <c r="BV19" t="s" s="42">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="BW19" s="41"/>
       <c r="BX19" s="41"/>
@@ -6022,7 +5969,7 @@
       <c r="CQ19" s="41"/>
       <c r="CR19" s="41"/>
       <c r="CS19" t="s" s="42">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="CT19" s="41"/>
       <c r="CU19" s="41"/>
@@ -6048,7 +5995,7 @@
       <c r="DO19" s="41"/>
       <c r="DP19" s="41"/>
       <c r="DQ19" t="s" s="42">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="DR19" s="41"/>
       <c r="DS19" s="41"/>
@@ -6085,7 +6032,7 @@
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="40">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
@@ -6100,7 +6047,7 @@
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
       <c r="N20" t="s" s="42">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O20" s="41"/>
       <c r="P20" s="41"/>
@@ -6166,7 +6113,7 @@
       <c r="BT20" s="41"/>
       <c r="BU20" s="41"/>
       <c r="BV20" t="s" s="42">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="BW20" s="41"/>
       <c r="BX20" s="41"/>
@@ -6191,7 +6138,7 @@
       <c r="CQ20" s="41"/>
       <c r="CR20" s="41"/>
       <c r="CS20" t="s" s="42">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="CT20" s="41"/>
       <c r="CU20" s="41"/>
@@ -6217,7 +6164,7 @@
       <c r="DO20" s="41"/>
       <c r="DP20" s="41"/>
       <c r="DQ20" t="s" s="42">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="DR20" s="41"/>
       <c r="DS20" s="41"/>
@@ -6254,7 +6201,7 @@
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="45">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B21" s="46"/>
       <c r="C21" s="46"/>
@@ -6269,7 +6216,7 @@
       <c r="L21" s="46"/>
       <c r="M21" s="46"/>
       <c r="N21" t="s" s="47">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O21" s="46"/>
       <c r="P21" s="46"/>
@@ -6290,7 +6237,7 @@
       <c r="AE21" s="46"/>
       <c r="AF21" s="46"/>
       <c r="AG21" t="s" s="47">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AH21" s="46"/>
       <c r="AI21" s="46"/>
@@ -6311,7 +6258,7 @@
       <c r="AX21" s="46"/>
       <c r="AY21" s="46"/>
       <c r="AZ21" t="s" s="47">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="BA21" s="46"/>
       <c r="BB21" s="46"/>
@@ -6335,7 +6282,7 @@
       <c r="BT21" s="46"/>
       <c r="BU21" s="46"/>
       <c r="BV21" t="s" s="47">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="BW21" s="46"/>
       <c r="BX21" s="46"/>
@@ -6360,7 +6307,7 @@
       <c r="CQ21" s="46"/>
       <c r="CR21" s="46"/>
       <c r="CS21" t="s" s="47">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="CT21" s="46"/>
       <c r="CU21" s="46"/>
@@ -6386,7 +6333,7 @@
       <c r="DO21" s="46"/>
       <c r="DP21" s="46"/>
       <c r="DQ21" t="s" s="47">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="DR21" s="46"/>
       <c r="DS21" s="46"/>
@@ -6423,7 +6370,7 @@
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="49">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B22" s="50"/>
       <c r="C22" s="50"/>
@@ -6580,7 +6527,7 @@
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" t="s" s="52">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B23" s="53"/>
       <c r="C23" s="53"/>
@@ -6595,7 +6542,7 @@
       <c r="L23" s="53"/>
       <c r="M23" s="53"/>
       <c r="N23" t="s" s="54">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O23" s="53"/>
       <c r="P23" s="53"/>
@@ -6616,7 +6563,7 @@
       <c r="AE23" s="53"/>
       <c r="AF23" s="53"/>
       <c r="AG23" t="s" s="54">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AH23" s="53"/>
       <c r="AI23" s="53"/>
@@ -6637,7 +6584,7 @@
       <c r="AX23" s="53"/>
       <c r="AY23" s="53"/>
       <c r="AZ23" t="s" s="54">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BA23" s="53"/>
       <c r="BB23" s="53"/>
@@ -6661,7 +6608,7 @@
       <c r="BT23" s="53"/>
       <c r="BU23" s="53"/>
       <c r="BV23" t="s" s="54">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="BW23" s="53"/>
       <c r="BX23" s="53"/>
@@ -6686,7 +6633,7 @@
       <c r="CQ23" s="53"/>
       <c r="CR23" s="53"/>
       <c r="CS23" t="s" s="54">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="CT23" s="53"/>
       <c r="CU23" s="53"/>
@@ -6712,7 +6659,7 @@
       <c r="DO23" s="53"/>
       <c r="DP23" s="53"/>
       <c r="DQ23" t="s" s="54">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="DR23" s="53"/>
       <c r="DS23" s="53"/>
@@ -6806,7 +6753,7 @@
       <c r="AX24" s="57"/>
       <c r="AY24" s="57"/>
       <c r="AZ24" t="s" s="59">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BA24" s="57"/>
       <c r="BB24" s="57"/>
@@ -6855,7 +6802,7 @@
       <c r="CQ24" s="57"/>
       <c r="CR24" s="57"/>
       <c r="CS24" t="s" s="59">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="CT24" s="57"/>
       <c r="CU24" s="57"/>
@@ -6916,7 +6863,7 @@
     </row>
     <row r="25" ht="25" customHeight="1">
       <c r="A25" t="s" s="49">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B25" s="50"/>
       <c r="C25" s="50"/>
@@ -7073,7 +7020,7 @@
     </row>
     <row r="26" ht="25" customHeight="1">
       <c r="A26" t="s" s="52">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
@@ -7088,7 +7035,7 @@
       <c r="L26" s="53"/>
       <c r="M26" s="53"/>
       <c r="N26" t="s" s="54">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O26" s="53"/>
       <c r="P26" s="53"/>
@@ -7109,7 +7056,7 @@
       <c r="AE26" s="53"/>
       <c r="AF26" s="53"/>
       <c r="AG26" t="s" s="54">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AH26" s="53"/>
       <c r="AI26" s="53"/>
@@ -7130,7 +7077,7 @@
       <c r="AX26" s="53"/>
       <c r="AY26" s="53"/>
       <c r="AZ26" t="s" s="54">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="BA26" s="53"/>
       <c r="BB26" s="53"/>
@@ -7154,7 +7101,7 @@
       <c r="BT26" s="53"/>
       <c r="BU26" s="53"/>
       <c r="BV26" t="s" s="54">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="BW26" s="53"/>
       <c r="BX26" s="53"/>
@@ -7179,7 +7126,7 @@
       <c r="CQ26" s="53"/>
       <c r="CR26" s="53"/>
       <c r="CS26" t="s" s="54">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="CT26" s="53"/>
       <c r="CU26" s="53"/>
@@ -7205,7 +7152,7 @@
       <c r="DO26" s="53"/>
       <c r="DP26" s="53"/>
       <c r="DQ26" t="s" s="54">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="DR26" s="53"/>
       <c r="DS26" s="53"/>
@@ -7299,7 +7246,7 @@
       <c r="AX27" s="62"/>
       <c r="AY27" s="62"/>
       <c r="AZ27" t="s" s="64">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="BA27" s="62"/>
       <c r="BB27" s="62"/>
@@ -7348,7 +7295,7 @@
       <c r="CQ27" s="62"/>
       <c r="CR27" s="62"/>
       <c r="CS27" t="s" s="64">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="CT27" s="62"/>
       <c r="CU27" s="62"/>
@@ -7409,7 +7356,7 @@
     </row>
     <row r="28" ht="25" customHeight="1">
       <c r="A28" t="s" s="21">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -7566,7 +7513,7 @@
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" t="s" s="67">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B29" s="68"/>
       <c r="C29" s="68"/>
@@ -7582,7 +7529,7 @@
       <c r="M29" s="68"/>
       <c r="N29" s="68"/>
       <c r="O29" t="s" s="69">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="P29" s="68"/>
       <c r="Q29" s="68"/>
@@ -7594,7 +7541,7 @@
       <c r="W29" s="68"/>
       <c r="X29" s="68"/>
       <c r="Y29" t="s" s="69">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="Z29" s="68"/>
       <c r="AA29" s="68"/>
@@ -7615,7 +7562,7 @@
       <c r="AP29" s="68"/>
       <c r="AQ29" s="68"/>
       <c r="AR29" t="s" s="69">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="AS29" s="68"/>
       <c r="AT29" s="68"/>
@@ -7626,7 +7573,7 @@
       <c r="AY29" s="68"/>
       <c r="AZ29" s="68"/>
       <c r="BA29" t="s" s="69">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="BB29" s="68"/>
       <c r="BC29" s="68"/>
@@ -7642,7 +7589,7 @@
       <c r="BM29" s="68"/>
       <c r="BN29" s="68"/>
       <c r="BO29" t="s" s="69">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="BP29" s="68"/>
       <c r="BQ29" s="68"/>
@@ -7655,7 +7602,7 @@
       <c r="BX29" s="68"/>
       <c r="BY29" s="68"/>
       <c r="BZ29" t="s" s="69">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="CA29" s="68"/>
       <c r="CB29" s="68"/>
@@ -7667,7 +7614,7 @@
       <c r="CH29" s="68"/>
       <c r="CI29" s="68"/>
       <c r="CJ29" t="s" s="69">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="CK29" s="68"/>
       <c r="CL29" s="68"/>
@@ -7684,7 +7631,7 @@
       <c r="CW29" s="68"/>
       <c r="CX29" s="68"/>
       <c r="CY29" t="s" s="69">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="CZ29" s="68"/>
       <c r="DA29" s="68"/>
@@ -7695,7 +7642,7 @@
       <c r="DF29" s="68"/>
       <c r="DG29" s="68"/>
       <c r="DH29" t="s" s="69">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="DI29" s="68"/>
       <c r="DJ29" s="68"/>
@@ -7712,7 +7659,7 @@
       <c r="DU29" s="68"/>
       <c r="DV29" s="68"/>
       <c r="DW29" t="s" s="69">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="DX29" s="68"/>
       <c r="DY29" s="68"/>
@@ -7727,7 +7674,7 @@
       <c r="EH29" s="68"/>
       <c r="EI29" s="68"/>
       <c r="EJ29" t="s" s="69">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="EK29" s="68"/>
       <c r="EL29" s="68"/>
@@ -7889,7 +7836,7 @@
       <c r="EM30" s="28"/>
       <c r="EN30" s="28"/>
       <c r="EO30" t="s" s="29">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="EP30" s="30"/>
       <c r="EQ30" s="30"/>
@@ -7904,7 +7851,7 @@
     </row>
     <row r="31" ht="25" customHeight="1">
       <c r="A31" t="s" s="13">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -8061,7 +8008,7 @@
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="A32" t="s" s="67">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B32" s="68"/>
       <c r="C32" s="68"/>
@@ -8085,7 +8032,7 @@
       <c r="U32" s="68"/>
       <c r="V32" s="68"/>
       <c r="W32" t="s" s="69">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="X32" s="68"/>
       <c r="Y32" s="68"/>
@@ -8103,7 +8050,7 @@
       <c r="AK32" s="68"/>
       <c r="AL32" s="68"/>
       <c r="AM32" t="s" s="69">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="AN32" s="68"/>
       <c r="AO32" s="68"/>
@@ -8123,7 +8070,7 @@
       <c r="BC32" s="68"/>
       <c r="BD32" s="68"/>
       <c r="BE32" t="s" s="69">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="BF32" s="68"/>
       <c r="BG32" s="68"/>
@@ -8149,7 +8096,7 @@
       <c r="CA32" s="68"/>
       <c r="CB32" s="68"/>
       <c r="CC32" t="s" s="69">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="CD32" s="68"/>
       <c r="CE32" s="68"/>
@@ -8163,7 +8110,7 @@
       <c r="CM32" s="68"/>
       <c r="CN32" s="68"/>
       <c r="CO32" t="s" s="69">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="CP32" s="68"/>
       <c r="CQ32" s="68"/>
@@ -8183,7 +8130,7 @@
       <c r="DE32" s="68"/>
       <c r="DF32" s="68"/>
       <c r="DG32" t="s" s="69">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="DH32" s="68"/>
       <c r="DI32" s="68"/>
@@ -8208,7 +8155,7 @@
       <c r="EB32" s="68"/>
       <c r="EC32" s="68"/>
       <c r="ED32" t="s" s="69">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="EE32" s="68"/>
       <c r="EF32" s="68"/>
@@ -8232,7 +8179,7 @@
     </row>
     <row r="33" ht="25" customHeight="1">
       <c r="A33" t="s" s="27">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B33" s="23"/>
       <c r="C33" s="23"/>
@@ -8389,7 +8336,7 @@
     </row>
     <row r="34" ht="30" customHeight="1">
       <c r="A34" t="s" s="67">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B34" s="68"/>
       <c r="C34" s="68"/>
@@ -8406,7 +8353,7 @@
       <c r="N34" s="68"/>
       <c r="O34" s="68"/>
       <c r="P34" t="s" s="69">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="Q34" s="68"/>
       <c r="R34" s="68"/>
@@ -8427,7 +8374,7 @@
       <c r="AG34" s="68"/>
       <c r="AH34" s="68"/>
       <c r="AI34" t="s" s="69">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AJ34" s="68"/>
       <c r="AK34" s="68"/>
@@ -8449,7 +8396,7 @@
       <c r="BA34" s="68"/>
       <c r="BB34" s="68"/>
       <c r="BC34" t="s" s="69">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="BD34" s="68"/>
       <c r="BE34" s="68"/>
@@ -8476,7 +8423,7 @@
       <c r="BZ34" s="68"/>
       <c r="CA34" s="68"/>
       <c r="CB34" t="s" s="69">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="CC34" s="68"/>
       <c r="CD34" s="68"/>
@@ -8502,7 +8449,7 @@
       <c r="CX34" s="68"/>
       <c r="CY34" s="68"/>
       <c r="CZ34" t="s" s="69">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="DA34" s="68"/>
       <c r="DB34" s="68"/>
@@ -8529,7 +8476,7 @@
       <c r="DW34" s="68"/>
       <c r="DX34" s="68"/>
       <c r="DY34" t="s" s="69">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="DZ34" s="68"/>
       <c r="EA34" s="68"/>
@@ -8558,7 +8505,7 @@
     </row>
     <row r="35" ht="25" customHeight="1">
       <c r="A35" t="s" s="27">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="23"/>
@@ -8715,7 +8662,7 @@
     </row>
     <row r="36" ht="30" customHeight="1">
       <c r="A36" t="s" s="67">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B36" s="68"/>
       <c r="C36" s="68"/>
@@ -8738,7 +8685,7 @@
       <c r="T36" s="68"/>
       <c r="U36" s="68"/>
       <c r="V36" t="s" s="69">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="W36" s="68"/>
       <c r="X36" s="68"/>
@@ -8755,7 +8702,7 @@
       <c r="AI36" s="68"/>
       <c r="AJ36" s="68"/>
       <c r="AK36" t="s" s="69">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AL36" s="68"/>
       <c r="AM36" s="68"/>
@@ -8768,7 +8715,7 @@
       <c r="AT36" s="68"/>
       <c r="AU36" s="68"/>
       <c r="AV36" t="s" s="69">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AW36" s="68"/>
       <c r="AX36" s="68"/>
@@ -8787,7 +8734,7 @@
       <c r="BK36" s="68"/>
       <c r="BL36" s="68"/>
       <c r="BM36" t="s" s="69">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="BN36" s="68"/>
       <c r="BO36" s="68"/>
@@ -8824,7 +8771,7 @@
       <c r="CT36" s="68"/>
       <c r="CU36" s="68"/>
       <c r="CV36" t="s" s="69">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="CW36" s="68"/>
       <c r="CX36" s="68"/>
@@ -8843,7 +8790,7 @@
       <c r="DK36" s="68"/>
       <c r="DL36" s="68"/>
       <c r="DM36" t="s" s="69">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="DN36" s="68"/>
       <c r="DO36" s="68"/>
@@ -8863,7 +8810,7 @@
       <c r="EC36" s="68"/>
       <c r="ED36" s="68"/>
       <c r="EE36" t="s" s="69">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="EF36" s="68"/>
       <c r="EG36" s="68"/>
@@ -8886,7 +8833,7 @@
     </row>
     <row r="37" ht="25" customHeight="1">
       <c r="A37" t="s" s="27">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B37" s="23"/>
       <c r="C37" s="23"/>
@@ -9043,7 +8990,7 @@
     </row>
     <row r="38" ht="30" customHeight="1">
       <c r="A38" t="s" s="67">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B38" s="68"/>
       <c r="C38" s="68"/>
@@ -9066,7 +9013,7 @@
       <c r="T38" s="68"/>
       <c r="U38" s="68"/>
       <c r="V38" t="s" s="69">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="W38" s="68"/>
       <c r="X38" s="68"/>
@@ -9083,7 +9030,7 @@
       <c r="AI38" s="68"/>
       <c r="AJ38" s="68"/>
       <c r="AK38" t="s" s="69">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AL38" s="68"/>
       <c r="AM38" s="68"/>
@@ -9096,7 +9043,7 @@
       <c r="AT38" s="68"/>
       <c r="AU38" s="68"/>
       <c r="AV38" t="s" s="69">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AW38" s="68"/>
       <c r="AX38" s="68"/>
@@ -9115,7 +9062,7 @@
       <c r="BK38" s="68"/>
       <c r="BL38" s="68"/>
       <c r="BM38" t="s" s="69">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="BN38" s="68"/>
       <c r="BO38" s="68"/>
@@ -9152,7 +9099,7 @@
       <c r="CT38" s="68"/>
       <c r="CU38" s="68"/>
       <c r="CV38" t="s" s="69">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="CW38" s="68"/>
       <c r="CX38" s="68"/>
@@ -9171,7 +9118,7 @@
       <c r="DK38" s="68"/>
       <c r="DL38" s="68"/>
       <c r="DM38" t="s" s="69">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="DN38" s="68"/>
       <c r="DO38" s="68"/>
@@ -9191,7 +9138,7 @@
       <c r="EC38" s="68"/>
       <c r="ED38" s="68"/>
       <c r="EE38" t="s" s="69">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="EF38" s="68"/>
       <c r="EG38" s="68"/>
@@ -9214,7 +9161,7 @@
     </row>
     <row r="39" ht="25" customHeight="1">
       <c r="A39" t="s" s="27">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B39" s="23"/>
       <c r="C39" s="23"/>
@@ -9371,7 +9318,7 @@
     </row>
     <row r="40" ht="30" customHeight="1">
       <c r="A40" t="s" s="67">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B40" s="68"/>
       <c r="C40" s="68"/>
@@ -9408,7 +9355,7 @@
       <c r="AH40" s="68"/>
       <c r="AI40" s="68"/>
       <c r="AJ40" t="s" s="69">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AK40" s="68"/>
       <c r="AL40" s="68"/>
@@ -9438,7 +9385,7 @@
       <c r="BJ40" s="68"/>
       <c r="BK40" s="68"/>
       <c r="BL40" t="s" s="69">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="BM40" s="68"/>
       <c r="BN40" s="68"/>
@@ -9475,7 +9422,7 @@
       <c r="CS40" s="68"/>
       <c r="CT40" s="68"/>
       <c r="CU40" t="s" s="69">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="CV40" s="68"/>
       <c r="CW40" s="68"/>
@@ -9494,7 +9441,7 @@
       <c r="DJ40" s="68"/>
       <c r="DK40" s="68"/>
       <c r="DL40" t="s" s="69">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="DM40" s="68"/>
       <c r="DN40" s="68"/>
@@ -9517,7 +9464,7 @@
       <c r="EE40" s="68"/>
       <c r="EF40" s="68"/>
       <c r="EG40" t="s" s="69">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="EH40" s="68"/>
       <c r="EI40" s="68"/>
@@ -9538,7 +9485,7 @@
     </row>
     <row r="41" ht="25" customHeight="1">
       <c r="A41" t="s" s="27">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="23"/>
@@ -9695,7 +9642,7 @@
     </row>
     <row r="42" ht="25" customHeight="1">
       <c r="A42" t="s" s="71">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B42" s="72"/>
       <c r="C42" s="72"/>
@@ -9729,7 +9676,7 @@
       <c r="AE42" s="72"/>
       <c r="AF42" s="72"/>
       <c r="AG42" t="s" s="73">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="AH42" s="72"/>
       <c r="AI42" s="72"/>
@@ -9854,7 +9801,7 @@
     </row>
     <row r="43" ht="14" customHeight="1">
       <c r="A43" t="s" s="75">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B43" s="76"/>
       <c r="C43" s="76"/>
@@ -9888,7 +9835,7 @@
       <c r="AE43" s="76"/>
       <c r="AF43" s="76"/>
       <c r="AG43" t="s" s="77">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AH43" s="76"/>
       <c r="AI43" s="76"/>
@@ -10157,7 +10104,7 @@
       <c r="EM44" s="28"/>
       <c r="EN44" s="28"/>
       <c r="EO44" t="s" s="29">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="EP44" s="30"/>
       <c r="EQ44" s="30"/>
@@ -10172,7 +10119,7 @@
     </row>
     <row r="45" ht="25" customHeight="1">
       <c r="A45" t="s" s="13">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -10329,7 +10276,7 @@
     </row>
     <row r="46" ht="25" customHeight="1">
       <c r="A46" t="s" s="79">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B46" s="80"/>
       <c r="C46" s="80"/>
@@ -10363,7 +10310,7 @@
       <c r="AE46" s="80"/>
       <c r="AF46" s="80"/>
       <c r="AG46" t="s" s="81">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AH46" s="80"/>
       <c r="AI46" s="80"/>
@@ -10488,7 +10435,7 @@
     </row>
     <row r="47" ht="14" customHeight="1">
       <c r="A47" t="s" s="83">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B47" s="84"/>
       <c r="C47" s="84"/>
@@ -10522,7 +10469,7 @@
       <c r="AE47" s="84"/>
       <c r="AF47" s="84"/>
       <c r="AG47" t="s" s="85">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="AH47" s="84"/>
       <c r="AI47" s="84"/>
@@ -10647,7 +10594,7 @@
     </row>
     <row r="48" ht="14" customHeight="1">
       <c r="A48" t="s" s="87">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B48" s="88"/>
       <c r="C48" s="88"/>
@@ -10681,7 +10628,7 @@
       <c r="AE48" s="88"/>
       <c r="AF48" s="88"/>
       <c r="AG48" t="s" s="89">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="AH48" s="88"/>
       <c r="AI48" s="88"/>
@@ -10806,7 +10753,7 @@
     </row>
     <row r="49" ht="14" customHeight="1">
       <c r="A49" t="s" s="87">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B49" s="88"/>
       <c r="C49" s="88"/>
@@ -10840,7 +10787,7 @@
       <c r="AE49" s="88"/>
       <c r="AF49" s="88"/>
       <c r="AG49" t="s" s="89">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="AH49" s="88"/>
       <c r="AI49" s="88"/>
@@ -10965,7 +10912,7 @@
     </row>
     <row r="50" ht="14" customHeight="1">
       <c r="A50" t="s" s="87">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B50" s="88"/>
       <c r="C50" s="88"/>
@@ -10999,7 +10946,7 @@
       <c r="AE50" s="88"/>
       <c r="AF50" s="88"/>
       <c r="AG50" t="s" s="89">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="AH50" s="88"/>
       <c r="AI50" s="88"/>
@@ -11124,7 +11071,7 @@
     </row>
     <row r="51" ht="14" customHeight="1">
       <c r="A51" t="s" s="87">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B51" s="88"/>
       <c r="C51" s="88"/>
@@ -11158,7 +11105,7 @@
       <c r="AE51" s="88"/>
       <c r="AF51" s="88"/>
       <c r="AG51" t="s" s="89">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AH51" s="88"/>
       <c r="AI51" s="88"/>
@@ -11283,7 +11230,7 @@
     </row>
     <row r="52" ht="14" customHeight="1">
       <c r="A52" t="s" s="87">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B52" s="88"/>
       <c r="C52" s="88"/>
@@ -11317,7 +11264,7 @@
       <c r="AE52" s="88"/>
       <c r="AF52" s="88"/>
       <c r="AG52" t="s" s="89">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AH52" s="88"/>
       <c r="AI52" s="88"/>
@@ -11442,7 +11389,7 @@
     </row>
     <row r="53" ht="14" customHeight="1">
       <c r="A53" t="s" s="87">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B53" s="88"/>
       <c r="C53" s="88"/>
@@ -11476,7 +11423,7 @@
       <c r="AE53" s="88"/>
       <c r="AF53" s="88"/>
       <c r="AG53" t="s" s="89">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AH53" s="88"/>
       <c r="AI53" s="88"/>
@@ -11601,7 +11548,7 @@
     </row>
     <row r="54" ht="14" customHeight="1">
       <c r="A54" t="s" s="87">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B54" s="88"/>
       <c r="C54" s="88"/>
@@ -11635,7 +11582,7 @@
       <c r="AE54" s="88"/>
       <c r="AF54" s="88"/>
       <c r="AG54" t="s" s="89">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AH54" s="88"/>
       <c r="AI54" s="88"/>
@@ -11760,7 +11707,7 @@
     </row>
     <row r="55" ht="14" customHeight="1">
       <c r="A55" t="s" s="87">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B55" s="88"/>
       <c r="C55" s="88"/>
@@ -11794,7 +11741,7 @@
       <c r="AE55" s="88"/>
       <c r="AF55" s="88"/>
       <c r="AG55" t="s" s="89">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="AH55" s="88"/>
       <c r="AI55" s="88"/>
@@ -11919,7 +11866,7 @@
     </row>
     <row r="56" ht="14" customHeight="1">
       <c r="A56" t="s" s="87">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B56" s="88"/>
       <c r="C56" s="88"/>
@@ -11953,7 +11900,7 @@
       <c r="AE56" s="88"/>
       <c r="AF56" s="88"/>
       <c r="AG56" t="s" s="89">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="AH56" s="88"/>
       <c r="AI56" s="88"/>
@@ -12078,7 +12025,7 @@
     </row>
     <row r="57" ht="15" customHeight="1">
       <c r="A57" t="s" s="91">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B57" s="92"/>
       <c r="C57" s="92"/>
@@ -12234,9 +12181,7 @@
       <c r="EW57" s="96"/>
     </row>
     <row r="58" ht="20" customHeight="1">
-      <c r="A58" t="s" s="97">
-        <v>135</v>
-      </c>
+      <c r="A58" s="97"/>
       <c r="B58" s="98"/>
       <c r="C58" s="98"/>
       <c r="D58" s="98"/>
@@ -12297,7 +12242,7 @@
       <c r="BG58" s="98"/>
       <c r="BH58" s="98"/>
       <c r="BI58" t="s" s="99">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="BJ58" s="100"/>
       <c r="BK58" s="100"/>
@@ -12393,9 +12338,7 @@
       <c r="EW58" s="2"/>
     </row>
     <row r="59" ht="20" customHeight="1">
-      <c r="A59" t="s" s="102">
-        <v>137</v>
-      </c>
+      <c r="A59" s="102"/>
       <c r="B59" s="103"/>
       <c r="C59" s="103"/>
       <c r="D59" s="103"/>
@@ -12456,7 +12399,7 @@
       <c r="BG59" s="103"/>
       <c r="BH59" s="103"/>
       <c r="BI59" t="s" s="99">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="BJ59" s="100"/>
       <c r="BK59" s="100"/>
@@ -12697,7 +12640,7 @@
       <c r="EM60" s="2"/>
       <c r="EN60" s="2"/>
       <c r="EO60" t="s" s="106">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="EP60" s="107"/>
       <c r="EQ60" s="107"/>

</xml_diff>